<commit_message>
Diego: arreglo de etiquetas y excel - Actualizadas: Comision, ofeerta y secretaria
</commit_message>
<xml_diff>
--- a/tesis.xlsx
+++ b/tesis.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="26">
   <si>
     <t>Titulo</t>
   </si>
@@ -83,17 +83,31 @@
   </si>
   <si>
     <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit.</t>
+  </si>
+  <si>
+    <t>2013-10-20</t>
+  </si>
+  <si>
+    <t>2013-10-21</t>
+  </si>
+  <si>
+    <t>2013-10-22</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="dd\-mm\-yy;@"/>
-  </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -121,11 +135,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:AJ8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,8 +592,8 @@
       <c r="R5" t="s">
         <v>22</v>
       </c>
-      <c r="S5" s="3">
-        <v>41325</v>
+      <c r="S5" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="T5" t="s">
         <v>20</v>
@@ -621,8 +636,8 @@
       <c r="O6" t="s">
         <v>19</v>
       </c>
-      <c r="S6" s="3">
-        <v>41315</v>
+      <c r="S6" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="T6" t="s">
         <v>20</v>
@@ -665,14 +680,15 @@
       <c r="O7" t="s">
         <v>19</v>
       </c>
-      <c r="S7" s="3">
-        <v>41294</v>
+      <c r="S7" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="T7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="S8" s="4"/>
       <c r="AJ8" s="2"/>
     </row>
   </sheetData>

</xml_diff>